<commit_message>
Clean-up enum sheet (remove mapping deprecation)
</commit_message>
<xml_diff>
--- a/src/voc4cat/templates/vocab/blank_1.0_min.xlsx
+++ b/src/voc4cat/templates/vocab/blank_1.0_min.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\MyProg\gh-nfdi4cat\voc4cat-tool\src\voc4cat\templates\vocab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-tool\src\voc4cat\templates\vocab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9050F09-0F02-40D0-A27E-FE3F03F7780B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D958D5E-DF0A-4FFF-8634-7B543E2F4BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="345" windowWidth="28260" windowHeight="16380" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12" yWindow="7188" windowWidth="23064" windowHeight="7224" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concept Scheme" sheetId="3" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="190">
   <si>
     <t>Template version</t>
   </si>
@@ -575,12 +575,6 @@
   </si>
   <si>
     <t>1.0.rev-2025-06a</t>
-  </si>
-  <si>
-    <t>Obsoletion Reason Mappings</t>
-  </si>
-  <si>
-    <t>This mapping was added in error.</t>
   </si>
   <si>
     <t>skos:broader,
@@ -941,7 +935,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1020,7 +1014,6 @@
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -1355,18 +1348,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{58381442-B18C-4348-B569-355AE6C4FF6C}" name="obsoletion_reason_map" displayName="obsoletion_reason_map" ref="C4:C8" totalsRowShown="0">
-  <autoFilter ref="C4:C8" xr:uid="{58381442-B18C-4348-B569-355AE6C4FF6C}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{D367E604-69CE-4058-A059-4ED41EC28044}" name="Obsoletion Reason Mappings"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6B7C8BEC-E429-4014-B655-697EFB7EFF36}" name="obsoletion_reason_col" displayName="obsoletion_reason_col" ref="E4:E8" totalsRowShown="0">
-  <autoFilter ref="E4:E8" xr:uid="{6B7C8BEC-E429-4014-B655-697EFB7EFF36}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6B7C8BEC-E429-4014-B655-697EFB7EFF36}" name="obsoletion_reason_col" displayName="obsoletion_reason_col" ref="C4:C8" totalsRowShown="0">
+  <autoFilter ref="C4:C8" xr:uid="{6B7C8BEC-E429-4014-B655-697EFB7EFF36}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{442E4487-208C-4445-AAEF-711FDC5FBE1F}" name="Obsoletion Reason Collections"/>
   </tableColumns>
@@ -1676,17 +1659,17 @@
   </sheetPr>
   <dimension ref="A1:E999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="64.140625" customWidth="1"/>
-    <col min="3" max="3" width="67.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="64.109375" customWidth="1"/>
+    <col min="3" max="3" width="67.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="35.25" customHeight="1">
@@ -1694,22 +1677,22 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15"/>
+    <row r="2" spans="1:5" ht="14.4"/>
     <row r="3" spans="1:5" ht="35.25" customHeight="1">
       <c r="A3" s="25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>134</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.8">
       <c r="A4" s="20" t="s">
         <v>0</v>
       </c>
@@ -1764,7 +1747,7 @@
       </c>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="14.4">
       <c r="A8" s="6" t="s">
         <v>134</v>
       </c>
@@ -1786,7 +1769,7 @@
         <v>102</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E9" s="24" t="s">
         <v>123</v>
@@ -1801,7 +1784,7 @@
         <v>103</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E10" s="24"/>
     </row>
@@ -1814,7 +1797,7 @@
         <v>101</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E11" s="24" t="s">
         <v>104</v>
@@ -1829,7 +1812,7 @@
         <v>122</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E12" s="24"/>
     </row>
@@ -1857,11 +1840,11 @@
         <v>122</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="14.4">
       <c r="A15" s="26" t="s">
         <v>138</v>
       </c>
@@ -2983,67 +2966,67 @@
   </sheetPr>
   <dimension ref="A1:O114"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="50.5546875" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
-    <col min="9" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
+    <col min="9" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
     <col min="12" max="13" width="27" customWidth="1"/>
-    <col min="14" max="14" width="21.28515625" customWidth="1"/>
+    <col min="14" max="14" width="21.33203125" customWidth="1"/>
     <col min="15" max="16" width="19" customWidth="1"/>
     <col min="17" max="17" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30">
+    <row r="1" spans="1:15" ht="28.8">
       <c r="A1" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="32" t="s">
-        <v>186</v>
+      <c r="F1" s="31" t="s">
+        <v>184</v>
       </c>
       <c r="L1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="M1" t="s">
+        <v>171</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="O1" t="s">
         <v>173</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="O1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="G2" s="27" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H2" s="27"/>
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
       <c r="K2" s="29" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L2" s="27" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="M2" s="28"/>
       <c r="N2" s="28"/>
       <c r="O2" s="28"/>
     </row>
-    <row r="3" spans="1:15" ht="30">
+    <row r="3" spans="1:15" ht="28.8">
       <c r="A3" t="s">
         <v>145</v>
       </c>
@@ -3057,7 +3040,7 @@
         <v>153</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>155</v>
@@ -3075,16 +3058,16 @@
         <v>158</v>
       </c>
       <c r="L3" t="s">
+        <v>179</v>
+      </c>
+      <c r="M3" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="N3" t="s">
+        <v>180</v>
+      </c>
+      <c r="O3" t="s">
         <v>181</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="N3" t="s">
-        <v>182</v>
-      </c>
-      <c r="O3" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="64.5" customHeight="1">
@@ -3107,10 +3090,10 @@
         <v>141</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I4" s="14" t="s">
         <v>138</v>
@@ -3125,7 +3108,7 @@
         <v>131</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>129</v>
@@ -4587,28 +4570,28 @@
   </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="40.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="8" width="26.28515625" customWidth="1"/>
-    <col min="9" max="9" width="42.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="40.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="7" max="8" width="26.33203125" customWidth="1"/>
+    <col min="9" max="9" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25">
+    <row r="1" spans="1:9" ht="23.4">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="30">
+    <row r="3" spans="1:9" ht="28.8">
       <c r="A3" s="18" t="s">
         <v>159</v>
       </c>
@@ -4867,26 +4850,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB86794-2A8B-4BE0-A9BC-E8B9B5C97189}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="6" width="32.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="32.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25">
+    <row r="1" spans="1:7" ht="23.4">
       <c r="A1" s="3" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="G2" s="27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4909,7 +4890,7 @@
         <v>151</v>
       </c>
       <c r="G3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="18" customFormat="1" ht="36.75" customHeight="1">
@@ -4934,30 +4915,6 @@
       <c r="G4" s="14" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="G5" s="30"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="G6" s="30"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="G7" s="30"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="G8" s="30"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="G9" s="30"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="G10" s="30"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="G11" s="30"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="G12" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -4978,23 +4935,23 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25">
+    <row r="1" spans="1:2" ht="23.4">
       <c r="A1" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2" ht="15">
+    <row r="2" spans="1:2" ht="14.4">
       <c r="A2" s="19" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15"/>
+    <row r="3" spans="1:2" ht="14.4"/>
     <row r="4" spans="1:2" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>20</v>
@@ -5258,86 +5215,78 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085DE69A-2A74-48F9-B963-10EA18647A12}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="60.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="5" max="5" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="35.25" customHeight="1">
+    <row r="1" spans="1:3" ht="35.25" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>98</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>95</v>
       </c>
-      <c r="E7" t="s">
+      <c r="C7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>96</v>
       </c>
-      <c r="E8" t="s">
+      <c r="C8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <tableParts count="3">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>